<commit_message>
Updated json handler , Utils
</commit_message>
<xml_diff>
--- a/resources/RUNNERFILE.xlsx
+++ b/resources/RUNNERFILE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makzarak\Desktop\Bench\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD030BE-267E-48B2-9925-05E5CB925AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230DACA1-B6AB-4D2D-8F54-08789401AF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A97F90B-5677-47E1-8EDD-AF691CC5D535}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -157,6 +157,27 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>ApiCalls</t>
+  </si>
+  <si>
+    <t>getSingleUserCall</t>
+  </si>
+  <si>
+    <t>postCreateUserCall</t>
+  </si>
+  <si>
+    <t>TC_014_GET_CALL</t>
+  </si>
+  <si>
+    <t>putUpdateUserCall</t>
+  </si>
+  <si>
+    <t>deleteUserCall</t>
   </si>
 </sst>
 </file>
@@ -207,10 +228,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC99E92-75B1-4388-8A79-80A56A3BF80F}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -595,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -902,15 +929,76 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified testcases and added extent spark reporter
</commit_message>
<xml_diff>
--- a/resources/RUNNERFILE.xlsx
+++ b/resources/RUNNERFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10D4ACA-791B-4C65-94E8-B19E8564478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D709BD4-1E6B-462F-8FF6-54BFF9618F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A97F90B-5677-47E1-8EDD-AF691CC5D535}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>TC_DATASHEET</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Web</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>test_language</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H2" sqref="H2:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,346 +588,346 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Modified testcases and log file
</commit_message>
<xml_diff>
--- a/resources/RUNNERFILE.xlsx
+++ b/resources/RUNNERFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D709BD4-1E6B-462F-8FF6-54BFF9618F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FD0AA8-900F-428C-B799-EE203004D241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A97F90B-5677-47E1-8EDD-AF691CC5D535}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+      <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,7 +600,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -615,7 +618,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -641,7 +644,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -649,7 +652,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -667,7 +670,7 @@
         <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -675,7 +678,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -693,7 +696,7 @@
         <v>24</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -719,7 +722,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -745,7 +748,7 @@
         <v>24</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -771,7 +774,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -797,7 +800,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -823,7 +826,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -849,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -857,7 +860,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -875,7 +878,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -883,7 +886,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -901,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -927,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Modified testcases and baseclass
</commit_message>
<xml_diff>
--- a/resources/RUNNERFILE.xlsx
+++ b/resources/RUNNERFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FD0AA8-900F-428C-B799-EE203004D241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F454DAA9-01D5-4E74-9F5C-AEEB1A04C5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A97F90B-5677-47E1-8EDD-AF691CC5D535}"/>
   </bookViews>
@@ -57,6 +57,9 @@
     <t>TC_DATASHEET</t>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>Web</t>
   </si>
   <si>
@@ -166,9 +169,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC99E92-75B1-4388-8A79-80A56A3BF80F}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,346 +591,346 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated listner class to add test type as category in report
</commit_message>
<xml_diff>
--- a/resources/RUNNERFILE.xlsx
+++ b/resources/RUNNERFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6A02AA-89A2-43E4-AB6B-2A3ABC41352A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8DC997-0734-41B3-ACBD-3842AE46014F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A97F90B-5677-47E1-8EDD-AF691CC5D535}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="55">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -199,15 +199,6 @@
   </si>
   <si>
     <t>go_to_new_release_page</t>
-  </si>
-  <si>
-    <t>CATEGORY</t>
-  </si>
-  <si>
-    <t>Smoke</t>
-  </si>
-  <si>
-    <t>Regression</t>
   </si>
 </sst>
 </file>
@@ -589,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC99E92-75B1-4388-8A79-80A56A3BF80F}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,10 +596,9 @@
     <col min="6" max="6" width="20.08984375" customWidth="1"/>
     <col min="7" max="7" width="19.1796875" customWidth="1"/>
     <col min="8" max="8" width="27.453125" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,11 +623,8 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
@@ -660,13 +647,10 @@
         <v>24</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>37</v>
       </c>
@@ -689,18 +673,15 @@
         <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -718,13 +699,10 @@
         <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -749,16 +727,13 @@
       <c r="H5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -776,13 +751,10 @@
         <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
@@ -805,13 +777,10 @@
         <v>24</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -834,18 +803,15 @@
         <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -865,16 +831,13 @@
       <c r="H9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -894,16 +857,13 @@
       <c r="H10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
@@ -923,11 +883,8 @@
       <c r="H11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
@@ -952,11 +909,8 @@
       <c r="H12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -981,11 +935,8 @@
       <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -1010,11 +961,8 @@
       <c r="H14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1039,16 +987,13 @@
       <c r="H15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1068,16 +1013,13 @@
       <c r="H16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -1097,16 +1039,13 @@
       <c r="H17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1126,16 +1065,13 @@
       <c r="H18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -1155,17 +1091,14 @@
       <c r="H19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed implicit waits in the testcases and updated listenets
</commit_message>
<xml_diff>
--- a/resources/RUNNERFILE.xlsx
+++ b/resources/RUNNERFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8DC997-0734-41B3-ACBD-3842AE46014F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32997EF-6621-4959-B857-D831FD768E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A97F90B-5677-47E1-8EDD-AF691CC5D535}"/>
   </bookViews>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC99E92-75B1-4388-8A79-80A56A3BF80F}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,7 +681,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -707,7 +707,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -759,7 +759,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
@@ -811,7 +811,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -837,7 +837,7 @@
         <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -863,7 +863,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
@@ -941,7 +941,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
@@ -967,7 +967,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -993,7 +993,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1019,7 +1019,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -1045,7 +1045,7 @@
         <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1071,7 +1071,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>

</xml_diff>